<commit_message>
Updated to make faster
</commit_message>
<xml_diff>
--- a/+aae550/+hw3/+p4/results.xlsx
+++ b/+aae550/+hw3/+p4/results.xlsx
@@ -100,8 +100,8 @@
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -504,34 +504,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -574,21 +559,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -873,7 +873,7 @@
   <dimension ref="B3:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +881,7 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -943,20 +943,20 @@
       <c r="D6" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="18" t="s">
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="49"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="42"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
@@ -966,35 +966,35 @@
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
       <c r="D7" s="48"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="21" t="s">
+      <c r="E7" s="50"/>
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="19" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="32" t="s">
+      <c r="J7" s="27" t="s">
         <v>11</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="36" t="s">
+      <c r="L7" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="40" t="s">
+      <c r="M7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="50" t="s">
+      <c r="O7" s="43" t="s">
         <v>8</v>
       </c>
       <c r="P7" s="1"/>
@@ -1004,41 +1004,41 @@
       <c r="C8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
-        <v>184</v>
+      <c r="D8" s="20">
+        <v>161</v>
       </c>
       <c r="E8" s="9">
-        <v>93240</v>
-      </c>
-      <c r="F8" s="22">
+        <v>62208</v>
+      </c>
+      <c r="F8" s="17">
         <v>3</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="20">
         <v>1</v>
       </c>
       <c r="H8" s="9">
         <v>1</v>
       </c>
-      <c r="I8" s="29">
+      <c r="I8" s="24">
         <v>4.2682799999999997E-4</v>
       </c>
-      <c r="J8" s="33">
+      <c r="J8" s="28">
         <v>1E-4</v>
       </c>
       <c r="K8" s="10">
         <v>1E-4</v>
       </c>
-      <c r="L8" s="37">
-        <v>16.415240000000001</v>
-      </c>
-      <c r="M8" s="41">
-        <v>-6.7790000000000001E-12</v>
-      </c>
-      <c r="N8" s="44">
-        <v>-2.3745836800000002</v>
+      <c r="L8" s="32">
+        <v>16.415247000000001</v>
+      </c>
+      <c r="M8" s="36">
+        <v>-2.64066E-7</v>
+      </c>
+      <c r="N8" s="39">
+        <v>-2.3745837559999998</v>
       </c>
       <c r="O8" s="11">
-        <v>-3.8242400000000001</v>
+        <v>-3.8242421499999999</v>
       </c>
       <c r="P8" s="1"/>
     </row>
@@ -1047,41 +1047,41 @@
       <c r="C9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="26">
-        <v>197</v>
+      <c r="D9" s="21">
+        <v>135</v>
       </c>
       <c r="E9" s="13">
-        <v>99792</v>
-      </c>
-      <c r="F9" s="23">
+        <v>62224</v>
+      </c>
+      <c r="F9" s="18">
         <v>3</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="21">
         <v>1</v>
       </c>
       <c r="H9" s="13">
         <v>1</v>
       </c>
-      <c r="I9" s="30">
-        <v>4.2683519999999999E-4</v>
-      </c>
-      <c r="J9" s="34">
-        <v>1.00005E-4</v>
+      <c r="I9" s="25">
+        <v>4.2682838582100001E-4</v>
+      </c>
+      <c r="J9" s="29">
+        <v>1E-4</v>
       </c>
       <c r="K9" s="14">
-        <v>1.00002E-4</v>
-      </c>
-      <c r="L9" s="38">
-        <v>16.415849000000001</v>
-      </c>
-      <c r="M9" s="42">
-        <v>-3.0456000000000001E-5</v>
-      </c>
-      <c r="N9" s="45">
-        <v>-2.3741354000000001</v>
+        <v>1E-4</v>
+      </c>
+      <c r="L9" s="33">
+        <v>16.415243353566702</v>
+      </c>
+      <c r="M9" s="37">
+        <v>-2.4861110000000001E-9</v>
+      </c>
+      <c r="N9" s="40">
+        <v>-2.3745835400000002</v>
       </c>
       <c r="O9" s="15">
-        <v>-3.8238146</v>
+        <v>-3.8242424000000002</v>
       </c>
       <c r="P9" s="1"/>
     </row>
@@ -1090,41 +1090,41 @@
       <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="27">
-        <v>203</v>
+      <c r="D10" s="22">
+        <v>126</v>
       </c>
       <c r="E10" s="3">
-        <v>102816</v>
-      </c>
-      <c r="F10" s="28">
+        <v>48768</v>
+      </c>
+      <c r="F10" s="23">
         <v>3</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="22">
         <v>1</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
       </c>
-      <c r="I10" s="31">
-        <v>4.2682838000000003E-4</v>
-      </c>
-      <c r="J10" s="35">
-        <v>1E-4</v>
+      <c r="I10" s="26">
+        <v>-4.5199415669999998E-4</v>
+      </c>
+      <c r="J10" s="30">
+        <v>1.3805937000000001E-4</v>
       </c>
       <c r="K10" s="6">
-        <v>1E-4</v>
-      </c>
-      <c r="L10" s="39">
-        <v>16.415243253290001</v>
-      </c>
-      <c r="M10" s="43">
-        <v>-3.0119000000000001E-12</v>
-      </c>
-      <c r="N10" s="46">
-        <v>-2.3745836854000002</v>
+        <v>1.4598512800000001E-4</v>
+      </c>
+      <c r="L10" s="34">
+        <v>17.125554000000001</v>
+      </c>
+      <c r="M10" s="38">
+        <v>-4.5199940000000003E-3</v>
+      </c>
+      <c r="N10" s="41">
+        <v>-1.62406568</v>
       </c>
       <c r="O10" s="7">
-        <v>-3.8242425</v>
+        <v>-3.185490202</v>
       </c>
       <c r="P10" s="1"/>
     </row>

</xml_diff>

<commit_message>
HW, thesis, old stuff.
</commit_message>
<xml_diff>
--- a/+aae550/+hw3/+p4/results.xlsx
+++ b/+aae550/+hw3/+p4/results.xlsx
@@ -873,7 +873,7 @@
   <dimension ref="B3:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="D8" s="20">
-        <v>161</v>
+        <v>224</v>
       </c>
       <c r="E8" s="9">
-        <v>62208</v>
+        <v>113400</v>
       </c>
       <c r="F8" s="17">
         <v>3</v>
@@ -1017,28 +1017,28 @@
         <v>1</v>
       </c>
       <c r="H8" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I8" s="24">
-        <v>4.2682799999999997E-4</v>
+        <v>4.0443380850999999E-4</v>
       </c>
       <c r="J8" s="28">
-        <v>1E-4</v>
+        <v>1.000016E-9</v>
       </c>
       <c r="K8" s="10">
-        <v>1E-4</v>
+        <v>1.5028780220000001E-4</v>
       </c>
       <c r="L8" s="32">
-        <v>16.415247000000001</v>
+        <v>16.888791281</v>
       </c>
       <c r="M8" s="36">
-        <v>-2.64066E-7</v>
+        <v>-2.8010999999999998E-12</v>
       </c>
       <c r="N8" s="39">
-        <v>-2.3745837559999998</v>
+        <v>-0.80774381747500001</v>
       </c>
       <c r="O8" s="11">
-        <v>-3.8242421499999999</v>
+        <v>-3.2082329999999999E-9</v>
       </c>
       <c r="P8" s="1"/>
     </row>
@@ -1048,10 +1048,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="21">
-        <v>135</v>
+        <v>257</v>
       </c>
       <c r="E9" s="13">
-        <v>62224</v>
+        <v>130032</v>
       </c>
       <c r="F9" s="18">
         <v>3</v>
@@ -1060,28 +1060,28 @@
         <v>1</v>
       </c>
       <c r="H9" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I9" s="25">
-        <v>4.2682838582100001E-4</v>
+        <v>4.0443380850199999E-4</v>
       </c>
       <c r="J9" s="29">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="K9" s="14">
-        <v>1E-4</v>
+        <v>1.5028780187200001E-4</v>
       </c>
       <c r="L9" s="33">
-        <v>16.415243353566702</v>
+        <v>16.88879127333</v>
       </c>
       <c r="M9" s="37">
-        <v>-2.4861110000000001E-9</v>
+        <v>-4.8209999999999998E-12</v>
       </c>
       <c r="N9" s="40">
-        <v>-2.3745835400000002</v>
+        <v>-0.80774382132926403</v>
       </c>
       <c r="O9" s="15">
-        <v>-3.8242424000000002</v>
+        <v>-1.03109E-9</v>
       </c>
       <c r="P9" s="1"/>
     </row>
@@ -1091,10 +1091,10 @@
         <v>2</v>
       </c>
       <c r="D10" s="22">
-        <v>126</v>
+        <v>260</v>
       </c>
       <c r="E10" s="3">
-        <v>48768</v>
+        <v>131544</v>
       </c>
       <c r="F10" s="23">
         <v>3</v>
@@ -1103,28 +1103,28 @@
         <v>1</v>
       </c>
       <c r="H10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="26">
-        <v>-4.5199415669999998E-4</v>
+        <v>4.0443380850700001E-4</v>
       </c>
       <c r="J10" s="30">
-        <v>1.3805937000000001E-4</v>
+        <v>1.000001E-9</v>
       </c>
       <c r="K10" s="6">
-        <v>1.4598512800000001E-4</v>
+        <v>1.5028780187399999E-4</v>
       </c>
       <c r="L10" s="34">
-        <v>17.125554000000001</v>
+        <v>16.888791273523101</v>
       </c>
       <c r="M10" s="38">
-        <v>-4.5199940000000003E-3</v>
+        <v>-1.7320000000000001E-11</v>
       </c>
       <c r="N10" s="41">
-        <v>-1.62406568</v>
+        <v>-0.80774382133240497</v>
       </c>
       <c r="O10" s="7">
-        <v>-3.185490202</v>
+        <v>-1.0430119999999999E-9</v>
       </c>
       <c r="P10" s="1"/>
     </row>

</xml_diff>